<commit_message>
Option to continue from a previous generation added.
</commit_message>
<xml_diff>
--- a/models/SWAT/economic_model/CS_input_data.xlsx
+++ b/models/SWAT/economic_model/CS_input_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\+PAPER_WORK+\Opti-Tool\CoMOLA_CS1_240503\models\SWAT\economic_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mstrauch\CoMOLA_OPTAIN_CS1\models\SWAT\economic_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF7257A-4BB9-435D-8196-96C1257C6BAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" tabRatio="901" activeTab="6" xr2:uid="{6C7E7271-B57A-4C5C-B27F-31DCFEB8A39E}"/>
+    <workbookView xWindow="-111" yWindow="-111" windowWidth="23271" windowHeight="12591" tabRatio="901" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="crop_prices" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">crop_prod_costs_mgt!$A$1:$D$90</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>enrico</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C26EF430-90FE-4E79-B63B-B27E56C55378}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,12 +61,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>enrico</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{A5F81E1D-6187-4E3C-8944-136386D62EC9}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,12 +85,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>enrico</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{DC18B395-E640-475C-9932-F105EF1A201F}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +100,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>euro/ha</t>
+          <t xml:space="preserve">euro/ha/year </t>
         </r>
       </text>
     </comment>
@@ -110,12 +109,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>enrico</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{1F0F60CE-698B-468B-BFE9-D932A4555747}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -134,12 +133,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>enrico</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D7933911-AE80-487C-8D36-E173EA103B8D}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -158,12 +157,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>enrico</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{FD574444-3D6F-4A97-8316-2D17235F9C49}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,32 +181,32 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{E366297C-62EA-42A8-B09A-F79192C34FFB}" keepAlive="1" name="Query - all_ops" description="Connessione alla query 'all_ops' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Query - all_ops" description="Connessione alla query 'all_ops' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=all_ops;Extended Properties=&quot;&quot;" command="SELECT * FROM [all_ops]"/>
   </connection>
-  <connection id="2" xr16:uid="{E3EC826B-5994-4963-A13A-8D33C5CCF99C}" keepAlive="1" name="Query - farmR_generic_CS9_HAYD" description="Connessione alla query 'farmR_generic_CS9_HAYD' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
+  <connection id="2" keepAlive="1" name="Query - farmR_generic_CS9_HAYD" description="Connessione alla query 'farmR_generic_CS9_HAYD' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=farmR_generic_CS9_HAYD;Extended Properties=&quot;&quot;" command="SELECT * FROM [farmR_generic_CS9_HAYD]"/>
   </connection>
-  <connection id="3" xr16:uid="{2EB5027B-36A7-4A6B-A28E-8BD3C042062F}" keepAlive="1" name="Query - farmR_generic_CS9_HAYD (2)" description="Connessione alla query 'farmR_generic_CS9_HAYD (2)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
+  <connection id="3" keepAlive="1" name="Query - farmR_generic_CS9_HAYD (2)" description="Connessione alla query 'farmR_generic_CS9_HAYD (2)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;farmR_generic_CS9_HAYD (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [farmR_generic_CS9_HAYD (2)]"/>
   </connection>
-  <connection id="4" xr16:uid="{3E4E38AB-1E40-45F6-8750-B87905E2D834}" keepAlive="1" name="Query - farmR_generic_CS9_HAYD (3)" description="Connessione alla query 'farmR_generic_CS9_HAYD (3)' nella cartella di lavoro." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="4" keepAlive="1" name="Query - farmR_generic_CS9_HAYD (3)" description="Connessione alla query 'farmR_generic_CS9_HAYD (3)' nella cartella di lavoro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;farmR_generic_CS9_HAYD (3)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [farmR_generic_CS9_HAYD (3)]"/>
   </connection>
-  <connection id="5" xr16:uid="{4840D1CE-E18C-4152-8D89-7E49F96DE2E6}" keepAlive="1" name="Query - mgt_crops_IRRV4" description="Connessione alla query 'mgt_crops_IRRV4' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
+  <connection id="5" keepAlive="1" name="Query - mgt_crops_IRRV4" description="Connessione alla query 'mgt_crops_IRRV4' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=mgt_crops_IRRV4;Extended Properties=&quot;&quot;" command="SELECT * FROM [mgt_crops_IRRV4]"/>
   </connection>
-  <connection id="6" xr16:uid="{6A51D645-6366-4572-9E5E-F2C58094F57E}" keepAlive="1" name="Query - mgt_crops_IRRV4 (2)" description="Connessione alla query 'mgt_crops_IRRV4 (2)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
+  <connection id="6" keepAlive="1" name="Query - mgt_crops_IRRV4 (2)" description="Connessione alla query 'mgt_crops_IRRV4 (2)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;mgt_crops_IRRV4 (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [mgt_crops_IRRV4 (2)]"/>
   </connection>
-  <connection id="7" xr16:uid="{72EAE802-CC89-432C-A454-B17DFBE9BB05}" keepAlive="1" name="Query - mgt_crops_IRRV4 (3)" description="Connessione alla query 'mgt_crops_IRRV4 (3)' nella cartella di lavoro." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="7" keepAlive="1" name="Query - mgt_crops_IRRV4 (3)" description="Connessione alla query 'mgt_crops_IRRV4 (3)' nella cartella di lavoro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;mgt_crops_IRRV4 (3)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [mgt_crops_IRRV4 (3)]"/>
   </connection>
-  <connection id="8" xr16:uid="{74C2867D-E082-420C-8669-E3B7173EA7EC}" keepAlive="1" name="Query - mgt_crops_IRRV4 (4)" description="Connessione alla query 'mgt_crops_IRRV4 (4)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
+  <connection id="8" keepAlive="1" name="Query - mgt_crops_IRRV4 (4)" description="Connessione alla query 'mgt_crops_IRRV4 (4)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;mgt_crops_IRRV4 (4)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [mgt_crops_IRRV4 (4)]"/>
   </connection>
-  <connection id="9" xr16:uid="{C3DA10FE-9A86-4C77-A7E6-E23550B19B77}" keepAlive="1" name="Query - mgt_crops_IRRV4 (5)" description="Connessione alla query 'mgt_crops_IRRV4 (5)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
+  <connection id="9" keepAlive="1" name="Query - mgt_crops_IRRV4 (5)" description="Connessione alla query 'mgt_crops_IRRV4 (5)' nella cartella di lavoro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;mgt_crops_IRRV4 (5)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [mgt_crops_IRRV4 (5)]"/>
   </connection>
 </connections>
@@ -432,12 +431,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>v. mgt</t>
-  </si>
-  <si>
-    <t>VALORE PER LOW TILL APPLICATO A TUTTE LE OPERAZIONI "TILL"</t>
-  </si>
-  <si>
     <t>field</t>
   </si>
   <si>
@@ -472,12 +465,18 @@
   </si>
   <si>
     <t>rnge like plant community</t>
+  </si>
+  <si>
+    <t>maintenance costs of the measure minus average annual production cost in the status quo (area-weighted average across status quo crops)</t>
+  </si>
+  <si>
+    <t>assumption of savings compared to normal till (labor cost and fuel savings because there is no deep ploughing operation in lowtill)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -810,10 +809,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Link" xfId="3" builtinId="8"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1124,23 +1123,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C014A0B0-3737-40C8-9858-1E193711460F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.4609375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.53515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.61328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
@@ -1154,7 +1153,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1170,7 +1169,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1182,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1196,7 +1195,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1209,7 +1208,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1222,7 +1221,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1235,7 +1234,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1248,7 +1247,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1261,7 +1260,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1277,7 +1276,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1290,7 +1289,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1306,7 +1305,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1319,7 +1318,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1333,7 +1332,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1349,7 +1348,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1365,7 +1364,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1378,7 +1377,7 @@
       <c r="G17" s="9"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B18" s="45"/>
       <c r="D18" s="41"/>
       <c r="E18" s="8"/>
@@ -1386,7 +1385,7 @@
       <c r="G18" s="9"/>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B19" s="45"/>
       <c r="D19" s="41"/>
       <c r="E19" s="8"/>
@@ -1394,7 +1393,7 @@
       <c r="G19" s="9"/>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B20" s="45"/>
       <c r="D20" s="41"/>
       <c r="E20" s="10"/>
@@ -1402,7 +1401,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B21" s="8"/>
       <c r="D21" s="41"/>
       <c r="E21" s="8"/>
@@ -1410,7 +1409,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B22" s="8"/>
       <c r="D22" s="41"/>
       <c r="E22" s="8"/>
@@ -1418,7 +1417,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B23" s="8"/>
       <c r="D23" s="41"/>
       <c r="E23" s="8"/>
@@ -1426,7 +1425,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B24" s="8"/>
       <c r="D24" s="41"/>
       <c r="E24" s="8"/>
@@ -1434,7 +1433,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B25" s="8"/>
       <c r="D25" s="41"/>
       <c r="E25" s="8"/>
@@ -1442,7 +1441,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="24"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B26" s="8"/>
       <c r="D26" s="41"/>
       <c r="E26" s="8"/>
@@ -1450,7 +1449,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="24"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B27" s="8"/>
       <c r="D27" s="41"/>
       <c r="E27" s="8"/>
@@ -1458,42 +1457,42 @@
       <c r="G27" s="9"/>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="9"/>
       <c r="H28" s="24"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="38"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="24"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="38"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
       <c r="H30" s="24"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="38"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="24"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="38"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="9"/>
       <c r="H32" s="24"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="38"/>
       <c r="D33" s="44"/>
       <c r="E33" s="8"/>
@@ -1501,37 +1500,37 @@
       <c r="G33" s="9"/>
       <c r="H33" s="24"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="38"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="38"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="38"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="38"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="38"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="38"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="38"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" s="38"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="38"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="38"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="38"/>
     </row>
   </sheetData>
@@ -1542,7 +1541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592DFE88-2666-4B2A-8C21-7B8FEE4069F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -1552,13 +1551,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1568,91 +1567,91 @@
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B2" s="6"/>
       <c r="C2" s="33"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B3" s="6"/>
       <c r="C3" s="33"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B4" s="46"/>
       <c r="C4" s="33"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B5" s="46"/>
       <c r="C5" s="33"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B6" s="46"/>
       <c r="C6" s="33"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B7" s="46"/>
       <c r="C7" s="33"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="48"/>
       <c r="B8" s="46"/>
       <c r="C8" s="33"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9" s="46"/>
       <c r="C9" s="33"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10" s="46"/>
       <c r="C10" s="33"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B11" s="46"/>
       <c r="C11" s="33"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B12" s="46"/>
       <c r="C12" s="33"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B13" s="46"/>
       <c r="C13" s="33"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="33"/>
       <c r="B14" s="46"/>
       <c r="C14" s="33"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="33"/>
       <c r="B15" s="46"/>
       <c r="C15" s="33"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="33"/>
       <c r="B16" s="46"/>
       <c r="C16" s="33"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="33"/>
       <c r="B17" s="46"/>
       <c r="C17" s="33"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="33"/>
       <c r="B18" s="46"/>
       <c r="C18" s="33"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="33"/>
       <c r="B19" s="46"/>
       <c r="C19" s="33"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="33"/>
       <c r="B20" s="46"/>
       <c r="C20" s="33"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C23" s="11"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1668,7 +1667,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17872EED-FD74-4E1E-B161-4509D7684307}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -1678,13 +1677,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1694,72 +1693,72 @@
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B4" s="46"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B5" s="46"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B6" s="46"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B7" s="46"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="48"/>
       <c r="B8" s="46"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9" s="46"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10" s="46"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B11" s="46"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B12" s="46"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B13" s="46"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="33"/>
       <c r="B14" s="47"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="33"/>
       <c r="B15" s="47"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="33"/>
       <c r="B16" s="47"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="33"/>
       <c r="B17" s="47"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="33"/>
       <c r="B18" s="47"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="33"/>
       <c r="B19" s="47"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="33"/>
       <c r="B20" s="47"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C23" s="11"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1775,19 +1774,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B99859-C5CF-46A6-8B7D-838DC8CD0A95}">
-  <dimension ref="A1:G108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="2" width="8.921875" style="3"/>
+    <col min="3" max="3" width="11.4609375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.921875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1817,11 +1818,8 @@
       <c r="D2">
         <v>85.47</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1835,7 +1833,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1849,7 +1847,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1866,7 +1864,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1880,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1897,7 +1895,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1928,7 +1926,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1945,7 +1943,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1959,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1973,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1987,7 +1985,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2001,7 +1999,7 @@
         <v>59.01</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2018,7 +2016,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -2032,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2046,7 +2044,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2063,7 +2061,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2080,7 +2078,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2094,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2108,7 +2106,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2125,7 +2123,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2139,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2153,7 +2151,7 @@
         <v>71.819999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2167,7 +2165,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2184,7 +2182,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2198,7 +2196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -2215,7 +2213,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2229,7 +2227,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2243,7 +2241,7 @@
         <v>43417</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2260,7 +2258,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2274,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -2291,7 +2289,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2305,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2322,7 +2320,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2336,7 +2334,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2350,7 +2348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -2364,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2378,7 +2376,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2392,7 +2390,7 @@
         <v>88.99</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2406,7 +2404,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2420,7 +2418,7 @@
         <v>32.9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2437,7 +2435,7 @@
         <v>-58</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2451,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2468,7 +2466,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -2482,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -2496,7 +2494,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -2510,7 +2508,7 @@
         <v>68145</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2524,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -2541,7 +2539,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -2555,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -2569,7 +2567,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -2583,7 +2581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -2597,7 +2595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -2611,7 +2609,7 @@
         <v>15750</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -2625,7 +2623,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -2639,7 +2637,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -2667,7 +2665,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -2681,7 +2679,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -2695,7 +2693,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -2709,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2723,7 +2721,7 @@
         <v>40.25</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>39</v>
       </c>
@@ -2740,7 +2738,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>41</v>
       </c>
@@ -2754,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>39</v>
       </c>
@@ -2771,7 +2769,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>41</v>
       </c>
@@ -2785,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -2799,7 +2797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -2813,7 +2811,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -2827,7 +2825,7 @@
         <v>64995</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -2841,7 +2839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>36</v>
       </c>
@@ -2855,7 +2853,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>36</v>
       </c>
@@ -2869,7 +2867,7 @@
         <v>62.7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -2883,7 +2881,7 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -2897,7 +2895,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -2911,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -2928,7 +2926,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>41</v>
       </c>
@@ -2942,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>36</v>
       </c>
@@ -2956,7 +2954,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>36</v>
       </c>
@@ -2970,7 +2968,7 @@
         <v>54.58</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>36</v>
       </c>
@@ -2984,7 +2982,7 @@
         <v>102.3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -2998,7 +2996,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -3012,7 +3010,7 @@
         <v>60038</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>36</v>
       </c>
@@ -3026,7 +3024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -3040,7 +3038,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>39</v>
       </c>
@@ -3057,7 +3055,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>36</v>
       </c>
@@ -3071,7 +3069,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>36</v>
       </c>
@@ -3085,7 +3083,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -3099,7 +3097,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>39</v>
       </c>
@@ -3116,94 +3114,30 @@
         <v>2447</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F93"/>
-      <c r="G93" s="28"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F94"/>
-      <c r="G94" s="28"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F95"/>
-      <c r="G95" s="28"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F96"/>
-      <c r="G96" s="28"/>
-    </row>
-    <row r="97" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F97"/>
-      <c r="G97" s="28"/>
-    </row>
-    <row r="98" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F98"/>
-      <c r="G98" s="28"/>
-    </row>
-    <row r="99" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F99"/>
-      <c r="G99" s="28"/>
-    </row>
-    <row r="100" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F100"/>
-      <c r="G100" s="28"/>
-    </row>
-    <row r="101" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F101"/>
-      <c r="G101" s="28"/>
-    </row>
-    <row r="102" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F102"/>
-      <c r="G102" s="28"/>
-    </row>
-    <row r="103" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F103"/>
-      <c r="G103" s="28"/>
-    </row>
-    <row r="104" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F104"/>
-      <c r="G104" s="28"/>
-    </row>
-    <row r="105" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F105"/>
-      <c r="G105" s="28"/>
-    </row>
-    <row r="106" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F106"/>
-      <c r="G106" s="28"/>
-    </row>
-    <row r="107" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F107"/>
-      <c r="G107" s="28"/>
-    </row>
-    <row r="108" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F108"/>
-      <c r="G108" s="27"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D90" xr:uid="{23B99859-C5CF-46A6-8B7D-838DC8CD0A95}"/>
+  <autoFilter ref="A1:D90"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDB7B77-0FF6-4C9C-9771-89C2CFCFA7F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.90625" style="29"/>
+    <col min="1" max="1" width="7.4609375" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.921875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="15.3828125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.921875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="31" t="s">
         <v>4</v>
       </c>
@@ -3214,7 +3148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3225,7 +3159,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3235,7 +3169,7 @@
       <c r="C3" s="25"/>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3246,7 +3180,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="35"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3255,7 +3189,7 @@
       </c>
       <c r="C5" s="26"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -3264,7 +3198,7 @@
       </c>
       <c r="C6" s="26"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3273,7 +3207,7 @@
       </c>
       <c r="C7" s="25"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3282,7 +3216,7 @@
       </c>
       <c r="C8" s="25"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3291,7 +3225,7 @@
       </c>
       <c r="C9" s="25"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3300,7 +3234,7 @@
       </c>
       <c r="C10" s="25"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -3309,7 +3243,7 @@
       </c>
       <c r="C11" s="25"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3320,7 +3254,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3329,7 +3263,7 @@
       </c>
       <c r="C13" s="25"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3339,7 +3273,7 @@
       <c r="C14" s="25"/>
       <c r="L14" s="35"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -3350,7 +3284,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3361,7 +3295,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3370,22 +3304,22 @@
       </c>
       <c r="C17" s="25"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="38"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="38"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="38"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="38"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="38"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="38"/>
     </row>
   </sheetData>
@@ -3394,22 +3328,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D957F356-540C-4BDB-AE15-BB2AD06F227A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.921875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="31" t="s">
         <v>4</v>
       </c>
@@ -3419,7 +3353,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3430,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3439,7 +3373,7 @@
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3448,7 +3382,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3457,7 +3391,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -3466,7 +3400,7 @@
       </c>
       <c r="C6" s="23"/>
     </row>
-    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3474,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3482,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3491,7 +3425,7 @@
       </c>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3500,7 +3434,7 @@
       </c>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -3508,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3516,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3524,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3532,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -3540,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3548,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3557,16 +3491,16 @@
       </c>
       <c r="C17"/>
     </row>
-    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="33"/>
       <c r="B18" s="28"/>
       <c r="C18"/>
     </row>
-    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="33"/>
       <c r="B19" s="28"/>
     </row>
-    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="33"/>
       <c r="B20" s="28"/>
     </row>
@@ -3577,26 +3511,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9FD6A9-730F-4C04-8803-921D1C40D78B}">
-  <dimension ref="A1:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" style="1"/>
-    <col min="5" max="6" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.90625" style="1"/>
+    <col min="3" max="3" width="10.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.921875" style="1"/>
+    <col min="5" max="6" width="11.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.921875" style="1"/>
     <col min="9" max="9" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="1"/>
+    <col min="10" max="16384" width="8.921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -3607,7 +3541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3615,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3623,7 +3557,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3632,48 +3566,39 @@
       </c>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="12">
-        <v>7407</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B6" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F14" s="12"/>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F13" s="12"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.4">
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.4">
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.4">
       <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.35">
-      <c r="I25" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3683,27 +3608,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3B52AB-11EB-43B9-867F-23C8F6C0C213}">
-  <dimension ref="A1:J25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.90625" style="1"/>
-    <col min="6" max="7" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.90625" style="1"/>
+    <col min="1" max="1" width="13.921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="116" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.921875" style="1"/>
+    <col min="6" max="7" width="11.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.921875" style="1"/>
     <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="1"/>
+    <col min="11" max="16384" width="8.921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -3714,85 +3639,90 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <f xml:space="preserve"> 25 - 921</f>
+        <v>-896</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="34">
-        <v>23460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <f>23460-921</f>
+        <v>22539</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="17">
+        <f>25-921</f>
+        <v>-896</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="21"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
       <c r="B5" s="34">
-        <v>0</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <f>27466-921</f>
+        <v>26545</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="34">
-        <v>27466</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B6" s="17">
+        <f>-53</f>
         <v>-53</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D7" s="12"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G14" s="12"/>
-    </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B8" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G13" s="12"/>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.4">
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.4">
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:10" x14ac:dyDescent="0.4">
       <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J25" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3802,23 +3732,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E73156-1BA8-441A-B151-1A3DEA08DD66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.90625" style="1"/>
-    <col min="5" max="5" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="13.921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.921875" style="1"/>
+    <col min="5" max="5" width="11.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -3829,7 +3759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3837,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3845,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3854,7 +3784,7 @@
       </c>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -3863,7 +3793,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3871,7 +3801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3879,7 +3809,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E14" s="12"/>
     </row>
   </sheetData>
@@ -3890,16 +3820,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFECE196-42F5-49B3-B817-D20007370838}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -3910,7 +3840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3921,7 +3851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3932,7 +3862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3943,7 +3873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3958,26 +3888,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FB4829-1243-479E-814D-2D1245331730}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.90625" style="1"/>
+    <col min="2" max="2" width="16.07421875" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.07421875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.53515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.4609375" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
@@ -3991,9 +3921,9 @@
       <c r="E1" s="50"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1">
         <v>0.1</v>
@@ -4001,7 +3931,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="52"/>
     </row>
-    <row r="3" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -4011,19 +3941,19 @@
       <c r="D3" s="51"/>
       <c r="E3" s="52"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1">
         <v>0.1</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4033,22 +3963,22 @@
       <c r="D5" s="51"/>
       <c r="E5" s="52"/>
     </row>
-    <row r="6" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="1">
         <v>0.1</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" s="51"/>
       <c r="E6" s="52"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="1">
         <v>0.9</v>
@@ -4056,7 +3986,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -4067,7 +3997,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -4077,9 +4007,9 @@
       <c r="C9" s="1"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" s="1">
         <v>0.9</v>
@@ -4087,9 +4017,9 @@
       <c r="C10" s="1"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1">
         <v>0.9</v>
@@ -4097,9 +4027,9 @@
       <c r="C11" s="1"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -4107,9 +4037,9 @@
       <c r="C12" s="1"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -4117,7 +4047,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -4127,9 +4057,9 @@
       <c r="C14" s="1"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -4137,18 +4067,18 @@
       <c r="C15" s="1"/>
       <c r="D15" s="51"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1">
         <v>0.9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -4157,7 +4087,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -4167,7 +4097,7 @@
       <c r="C18" s="1"/>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -4177,68 +4107,68 @@
       <c r="C19" s="1"/>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20"/>
       <c r="B20" s="54"/>
       <c r="E20" s="30"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21"/>
       <c r="B21" s="54"/>
       <c r="E21" s="30"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22"/>
       <c r="B22" s="54"/>
       <c r="C22" s="55"/>
       <c r="E22" s="30"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23"/>
       <c r="B23" s="54"/>
       <c r="E23" s="30"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24"/>
       <c r="B24" s="54"/>
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
       <c r="F25" s="31"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
       <c r="F26" s="31"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
       <c r="F27" s="31"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="1"/>
       <c r="B28" s="56"/>
       <c r="F28" s="31"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
       <c r="F29" s="31"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="1"/>
       <c r="B30" s="56"/>
       <c r="F30" s="31"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="56"/>
       <c r="F31" s="31"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="F32" s="31"/>
     </row>
   </sheetData>

</xml_diff>